<commit_message>
fix: last annotation position
</commit_message>
<xml_diff>
--- a/templates/test.xlsx
+++ b/templates/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,52 +481,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>#e975db58-5297-4119-945b-4923f6c217bd</t>
+          <t>#caff2b0e-3932-429f-b2fb-fc53d3980941</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="E2" t="n">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F2" t="n">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G2" t="n">
         <v>36</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>#ecfc5199-3e1f-4ebd-9033-69dba7d582cb</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>1264</v>
-      </c>
-      <c r="E3" t="n">
-        <v>359</v>
-      </c>
-      <c r="F3" t="n">
-        <v>113</v>
-      </c>
-      <c r="G3" t="n">
-        <v>42</v>
-      </c>
-      <c r="H3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>